<commit_message>
Add ip, fix bug, update excel files
</commit_message>
<xml_diff>
--- a/backend/database/PostgreSQL-caesb.xlsx
+++ b/backend/database/PostgreSQL-caesb.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fs\sinfra\COEMANT\SEPLAG\CMMS\Banco de dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hzlopes\Desktop\repositories\cmms\backend\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120" tabRatio="875" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120" tabRatio="875" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="pre-raw" sheetId="1" r:id="rId1"/>
@@ -379,9 +379,6 @@
     <t>END IF;</t>
   </si>
   <si>
-    <t>TE 20170002</t>
-  </si>
-  <si>
     <t>309D-000-000</t>
   </si>
   <si>
@@ -461,6 +458,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>TE 20170014</t>
   </si>
 </sst>
 </file>
@@ -53856,10 +53856,10 @@
         <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -54090,10 +54090,10 @@
         <v>PRIMARY KEY (med, aamm)</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -54101,10 +54101,10 @@
         <v>87</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -54170,10 +54170,10 @@
         <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -54185,8 +54185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54585,7 +54585,7 @@
         <v>66</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>65</v>
@@ -54595,7 +54595,7 @@
       </c>
       <c r="I15" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO caesb_meters VALUES (214, '008.535-9', 'Setor de Clubes Norte - Clube do Servidor', 'TE 20170002', 'A09S359813', 4);</v>
+        <v>INSERT INTO caesb_meters VALUES (214, '008.535-9', 'Setor de Clubes Norte - Clube do Servidor', 'TE 20170014', 'A09S359813', 4);</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -54615,7 +54615,7 @@
         <v>201</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I18" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B18,", '",C18,"');")</f>
@@ -54628,7 +54628,7 @@
         <v>202</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I19" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B19,", '",C19,"');")</f>
@@ -54641,7 +54641,7 @@
         <v>203</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I20" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B20,", '",C20,"');")</f>
@@ -54654,7 +54654,7 @@
         <v>204</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I21" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B21,", '",C21,"');")</f>
@@ -54667,7 +54667,7 @@
         <v>205</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I22" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B22,", '",C22,"');")</f>
@@ -54680,7 +54680,7 @@
         <v>206</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I23" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B23,", '",C23,"');")</f>
@@ -54693,7 +54693,7 @@
         <v>207</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I24" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B24,", '",C24,"');")</f>
@@ -54706,7 +54706,7 @@
         <v>207</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I25" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B25,", '",C25,"');")</f>
@@ -54719,7 +54719,7 @@
         <v>207</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I26" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B26,", '",C26,"');")</f>
@@ -54732,7 +54732,7 @@
         <v>207</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I27" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B27,", '",C27,"');")</f>
@@ -54745,7 +54745,7 @@
         <v>207</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I28" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B28,", '",C28,"');")</f>
@@ -54758,7 +54758,7 @@
         <v>207</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I29" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B29,", '",C29,"');")</f>
@@ -54771,7 +54771,7 @@
         <v>207</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I30" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B30,", '",C30,"');")</f>
@@ -54784,7 +54784,7 @@
         <v>207</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I31" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B31,", '",C31,"');")</f>
@@ -54797,7 +54797,7 @@
         <v>208</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I32" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B32,", '",C32,"');")</f>
@@ -54810,7 +54810,7 @@
         <v>208</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I33" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B33,", '",C33,"');")</f>
@@ -54822,7 +54822,7 @@
         <v>209</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I34" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B34,", '",C34,"');")</f>
@@ -54835,7 +54835,7 @@
         <v>210</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I35" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B35,", '",C35,"');")</f>
@@ -54848,7 +54848,7 @@
         <v>210</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I36" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B36,", '",C36,"');")</f>
@@ -54861,7 +54861,7 @@
         <v>210</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I37" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B37,", '",C37,"');")</f>
@@ -54874,7 +54874,7 @@
         <v>211</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I38" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B38,", '",C38,"');")</f>
@@ -54887,7 +54887,7 @@
         <v>212</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I39" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B39,", '",C39,"');")</f>
@@ -54900,7 +54900,7 @@
         <v>212</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I40" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B40,", '",C40,"');")</f>
@@ -54913,7 +54913,7 @@
         <v>213</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I41" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B41,", '",C41,"');")</f>
@@ -54926,7 +54926,7 @@
         <v>213</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I42" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B42,", '",C42,"');")</f>
@@ -54939,7 +54939,7 @@
         <v>214</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I43" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B43,", '",C43,"');")</f>
@@ -57449,10 +57449,10 @@
         <v>103</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -57460,10 +57460,10 @@
         <v>104</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -57472,10 +57472,10 @@
         <v>a.med,</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -57484,10 +57484,10 @@
         <v>a.id,</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -57496,10 +57496,10 @@
         <v>a.nome,</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -57508,10 +57508,10 @@
         <v>a.contrato,</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -57520,10 +57520,10 @@
         <v>a.hidrom,</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -57532,10 +57532,10 @@
         <v>a.cat,</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -57544,10 +57544,10 @@
         <v>ARRAY(SELECT b.asset_id FROM caesb_meters_assets AS b WHERE b.med = a.med) AS locais</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -57556,10 +57556,10 @@
         <v>ORDER BY a.med;</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -57567,10 +57567,10 @@
         <v>105</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -57582,7 +57582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -57610,10 +57610,10 @@
         <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -57625,7 +57625,7 @@
         <v>caesb_data</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -57662,7 +57662,7 @@
         <v>caesb_data</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -57671,10 +57671,10 @@
         <v>WHERE med = $1 AND aamm BETWEEN $2 AND $3 ORDER BY caesb_data.aamm;</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -57682,10 +57682,10 @@
         <v>113</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -57693,10 +57693,10 @@
         <v>105</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add STABLE attribute to get_ceb_bills and get_caesb_bills functions
</commit_message>
<xml_diff>
--- a/backend/database/PostgreSQL-caesb.xlsx
+++ b/backend/database/PostgreSQL-caesb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120" tabRatio="875" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120" tabRatio="875" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="pre-raw" sheetId="1" r:id="rId1"/>
@@ -346,9 +346,6 @@
     <t>)</t>
   </si>
   <si>
-    <t>LANGUAGE plpgsql AS $$ BEGIN</t>
-  </si>
-  <si>
     <t>RETURN QUERY SELECT</t>
   </si>
   <si>
@@ -461,6 +458,9 @@
   </si>
   <si>
     <t>TE 20170014</t>
+  </si>
+  <si>
+    <t>LANGUAGE plpgsql STABLE AS $$ BEGIN</t>
   </si>
 </sst>
 </file>
@@ -53856,10 +53856,10 @@
         <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -54090,10 +54090,10 @@
         <v>PRIMARY KEY (med, aamm)</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -54101,10 +54101,10 @@
         <v>87</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -54170,10 +54170,10 @@
         <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -54585,7 +54585,7 @@
         <v>66</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>65</v>
@@ -54615,7 +54615,7 @@
         <v>201</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I18" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B18,", '",C18,"');")</f>
@@ -54628,7 +54628,7 @@
         <v>202</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I19" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B19,", '",C19,"');")</f>
@@ -54641,7 +54641,7 @@
         <v>203</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I20" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B20,", '",C20,"');")</f>
@@ -54654,7 +54654,7 @@
         <v>204</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I21" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B21,", '",C21,"');")</f>
@@ -54667,7 +54667,7 @@
         <v>205</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I22" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B22,", '",C22,"');")</f>
@@ -54680,7 +54680,7 @@
         <v>206</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I23" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B23,", '",C23,"');")</f>
@@ -54693,7 +54693,7 @@
         <v>207</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I24" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B24,", '",C24,"');")</f>
@@ -54706,7 +54706,7 @@
         <v>207</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I25" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B25,", '",C25,"');")</f>
@@ -54719,7 +54719,7 @@
         <v>207</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I26" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B26,", '",C26,"');")</f>
@@ -54732,7 +54732,7 @@
         <v>207</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I27" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B27,", '",C27,"');")</f>
@@ -54745,7 +54745,7 @@
         <v>207</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I28" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B28,", '",C28,"');")</f>
@@ -54758,7 +54758,7 @@
         <v>207</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I29" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B29,", '",C29,"');")</f>
@@ -54771,7 +54771,7 @@
         <v>207</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I30" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B30,", '",C30,"');")</f>
@@ -54784,7 +54784,7 @@
         <v>207</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I31" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B31,", '",C31,"');")</f>
@@ -54797,7 +54797,7 @@
         <v>208</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I32" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B32,", '",C32,"');")</f>
@@ -54810,7 +54810,7 @@
         <v>208</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I33" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B33,", '",C33,"');")</f>
@@ -54822,7 +54822,7 @@
         <v>209</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I34" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B34,", '",C34,"');")</f>
@@ -54835,7 +54835,7 @@
         <v>210</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I35" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B35,", '",C35,"');")</f>
@@ -54848,7 +54848,7 @@
         <v>210</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I36" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B36,", '",C36,"');")</f>
@@ -54861,7 +54861,7 @@
         <v>210</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I37" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B37,", '",C37,"');")</f>
@@ -54874,7 +54874,7 @@
         <v>211</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I38" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B38,", '",C38,"');")</f>
@@ -54887,7 +54887,7 @@
         <v>212</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I39" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B39,", '",C39,"');")</f>
@@ -54900,7 +54900,7 @@
         <v>212</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I40" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B40,", '",C40,"');")</f>
@@ -54913,7 +54913,7 @@
         <v>213</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I41" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B41,", '",C41,"');")</f>
@@ -54926,7 +54926,7 @@
         <v>213</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I42" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B42,", '",C42,"');")</f>
@@ -54939,7 +54939,7 @@
         <v>214</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I43" s="5" t="str">
         <f>CONCATENATE("INSERT INTO ",'create-caesb_meters_assets'!$B$1," VALUES (",B43,", '",C43,"');")</f>
@@ -57332,8 +57332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57446,24 +57446,24 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -57472,10 +57472,10 @@
         <v>a.med,</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -57484,10 +57484,10 @@
         <v>a.id,</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -57496,10 +57496,10 @@
         <v>a.nome,</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -57508,10 +57508,10 @@
         <v>a.contrato,</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -57520,10 +57520,10 @@
         <v>a.hidrom,</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -57532,10 +57532,10 @@
         <v>a.cat,</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -57544,10 +57544,10 @@
         <v>ARRAY(SELECT b.asset_id FROM caesb_meters_assets AS b WHERE b.med = a.med) AS locais</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -57556,10 +57556,10 @@
         <v>FROM caesb_meters AS a</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -57568,21 +57568,21 @@
         <v>ORDER BY a.med;</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -57594,8 +57594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57607,10 +57607,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C1" s="5" t="str">
         <f>CONCATENATE("(",'create-caesb_data'!B2,", ",'create-caesb_data'!B3,", ",'create-caesb_data'!B3,") RETURNS SETOF ",'create-caesb_data'!B1)</f>
@@ -57619,42 +57619,42 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" s="5" t="str">
         <f>'create-caesb_data'!B1</f>
         <v>caesb_data</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="5" t="str">
         <f>'create-caesb_data'!A3</f>
         <v>aamm</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="5" t="str">
         <f>CONCATENATE('create-caesb_data'!B1,".",'create-caesb_data'!A2,", ")</f>
@@ -57667,14 +57667,14 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" s="5" t="str">
         <f>'create-caesb_data'!B1</f>
         <v>caesb_data</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -57683,32 +57683,32 @@
         <v>WHERE med = $1 AND aamm BETWEEN $2 AND $3 ORDER BY caesb_data.aamm;</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>